<commit_message>
Added previous Workloads to repeat.
</commit_message>
<xml_diff>
--- a/notes/BenchmarkResults - Total Run Time.xlsx
+++ b/notes/BenchmarkResults - Total Run Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navolskyi/Documents/Universitaet/BachelorThesis/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DFBE30-8868-8049-A8F4-CC930BA36D83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AFD8C3-7FC6-554A-98E7-2FC3DA092709}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12200" windowHeight="18000" activeTab="2" xr2:uid="{129C3D52-BAD1-6E42-9DB9-3123D8C679A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12880" windowHeight="18000" activeTab="2" xr2:uid="{129C3D52-BAD1-6E42-9DB9-3123D8C679A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ApacheJena" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="OrientDB" sheetId="2" r:id="rId3"/>
     <sheet name="Sparksee" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2094,7 +2094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FB19B8-25DC-1046-869A-DB575E87635F}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Filled introduction of thesis.
</commit_message>
<xml_diff>
--- a/notes/BenchmarkResults - Total Run Time.xlsx
+++ b/notes/BenchmarkResults - Total Run Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navolskyi/Documents/Universitaet/BachelorThesis/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F36B218-C3DC-1040-BB03-2E0A4BE79E13}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FD1903-4008-9441-A1C0-4985C4CC0B2F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="22800" windowHeight="17540" activeTab="2" xr2:uid="{129C3D52-BAD1-6E42-9DB9-3123D8C679A8}"/>
+    <workbookView xWindow="-11060" yWindow="-21600" windowWidth="22560" windowHeight="21600" xr2:uid="{129C3D52-BAD1-6E42-9DB9-3123D8C679A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ApacheJena" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="28">
   <si>
     <t>Node Count</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -468,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143DC56F-02E2-2049-98AA-BD30982A8091}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,56 +702,146 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
+      <c r="C14">
+        <v>2376160</v>
+      </c>
+      <c r="D14">
+        <v>2907899</v>
+      </c>
+      <c r="E14">
+        <v>3094397</v>
+      </c>
+      <c r="F14">
+        <v>3846024</v>
+      </c>
+      <c r="G14">
+        <v>5910883</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>2</v>
       </c>
+      <c r="C15">
+        <v>2433332</v>
+      </c>
+      <c r="D15">
+        <v>3025117</v>
+      </c>
+      <c r="E15">
+        <v>3124624</v>
+      </c>
+      <c r="F15">
+        <v>3813462</v>
+      </c>
+      <c r="G15">
+        <v>6063705</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="C16">
+        <v>2442656</v>
+      </c>
+      <c r="D16">
+        <v>3012931</v>
+      </c>
+      <c r="E16">
+        <v>3081916</v>
+      </c>
+      <c r="F16">
+        <v>3698494</v>
+      </c>
+      <c r="G16">
+        <v>5899016</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="e">
+      <c r="C17" s="2">
         <f>SUM(C14:C16)/COUNT(C14:C16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="2" t="e">
+        <v>40.28971111111111</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" ref="D17:G17" si="2">SUM(D14:D16)/COUNT(D14:D16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="2" t="e">
+        <v>49.699705555555553</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="2" t="e">
+        <v>51.67187222222222</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="2" t="e">
+        <v>63.099888888888891</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>99.297800000000009</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6125840</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2">
+        <v>6258567</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>3</v>
       </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="2">
+        <v>6333108</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -767,9 +863,9 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="2" t="e">
+      <c r="G21" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>103.98619444444445</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -799,6 +895,9 @@
       <c r="C25" t="s">
         <v>25</v>
       </c>
+      <c r="D25">
+        <v>967970</v>
+      </c>
       <c r="E25" t="s">
         <v>25</v>
       </c>
@@ -816,6 +915,9 @@
       <c r="C26" t="s">
         <v>25</v>
       </c>
+      <c r="D26">
+        <v>1000083</v>
+      </c>
       <c r="E26" t="s">
         <v>25</v>
       </c>
@@ -833,6 +935,9 @@
       <c r="C27" t="s">
         <v>25</v>
       </c>
+      <c r="D27">
+        <v>1050479</v>
+      </c>
       <c r="E27" t="s">
         <v>25</v>
       </c>
@@ -851,9 +956,9 @@
         <f>SUM(C25:C27)/COUNT(C25:C27)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="2" t="e">
+      <c r="D28" s="2">
         <f t="shared" ref="D28:G28" si="4">SUM(D25:D27)/COUNT(D25:D27)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>16.769622222222225</v>
       </c>
       <c r="E28" s="2" t="e">
         <f t="shared" si="4"/>
@@ -1085,6 +1190,9 @@
       <c r="C43" t="s">
         <v>25</v>
       </c>
+      <c r="D43">
+        <v>2465830</v>
+      </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
@@ -1102,6 +1210,9 @@
       <c r="C44" t="s">
         <v>25</v>
       </c>
+      <c r="D44">
+        <v>2536271</v>
+      </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
@@ -1119,6 +1230,9 @@
       <c r="C45" t="s">
         <v>25</v>
       </c>
+      <c r="D45">
+        <v>2437063</v>
+      </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
@@ -1137,9 +1251,9 @@
         <f>SUM(C43:C45)/COUNT(C43:C45)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D46" s="2" t="e">
+      <c r="D46" s="2">
         <f t="shared" ref="D46:G46" si="7">SUM(D43:D45)/COUNT(D43:D45)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>41.328688888888891</v>
       </c>
       <c r="E46" s="2" t="e">
         <f t="shared" si="7"/>
@@ -1161,6 +1275,9 @@
       <c r="C47" t="s">
         <v>25</v>
       </c>
+      <c r="D47" s="2">
+        <v>2277197</v>
+      </c>
       <c r="E47" t="s">
         <v>25</v>
       </c>
@@ -1178,6 +1295,9 @@
       <c r="C48" t="s">
         <v>25</v>
       </c>
+      <c r="D48" s="2">
+        <v>2643446</v>
+      </c>
       <c r="E48" t="s">
         <v>25</v>
       </c>
@@ -1195,6 +1315,9 @@
       <c r="C49" t="s">
         <v>25</v>
       </c>
+      <c r="D49" s="2">
+        <v>2582408</v>
+      </c>
       <c r="E49" t="s">
         <v>25</v>
       </c>
@@ -1213,9 +1336,9 @@
         <f>SUM(C47:C49)/COUNT(C47:C49)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D50" s="2" t="e">
+      <c r="D50" s="2">
         <f t="shared" ref="D50:G50" si="8">SUM(D47:D49)/COUNT(D47:D49)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>41.683616666666666</v>
       </c>
       <c r="E50" s="2" t="e">
         <f t="shared" si="8"/>
@@ -1237,6 +1360,9 @@
       <c r="C51" t="s">
         <v>25</v>
       </c>
+      <c r="D51" s="2">
+        <v>2647911</v>
+      </c>
       <c r="E51" t="s">
         <v>25</v>
       </c>
@@ -1254,6 +1380,9 @@
       <c r="C52" t="s">
         <v>25</v>
       </c>
+      <c r="D52" s="2">
+        <v>2670894</v>
+      </c>
       <c r="E52" t="s">
         <v>25</v>
       </c>
@@ -1271,6 +1400,9 @@
       <c r="C53" t="s">
         <v>25</v>
       </c>
+      <c r="D53" s="2">
+        <v>2597951</v>
+      </c>
       <c r="E53" t="s">
         <v>25</v>
       </c>
@@ -1289,9 +1421,9 @@
         <f>SUM(C51:C53)/COUNT(C51:C53)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D54" s="2" t="e">
+      <c r="D54" s="2">
         <f t="shared" ref="D54:G54" si="9">SUM(D51:D53)/COUNT(D51:D53)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>43.981977777777772</v>
       </c>
       <c r="E54" s="2" t="e">
         <f t="shared" si="9"/>
@@ -1320,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5871CBE7-73D2-3641-9208-02FB5774B726}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1554,56 +1686,146 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
+      <c r="C14">
+        <v>2170317</v>
+      </c>
+      <c r="D14">
+        <v>3133499</v>
+      </c>
+      <c r="E14">
+        <v>2755878</v>
+      </c>
+      <c r="F14">
+        <v>2886937</v>
+      </c>
+      <c r="G14">
+        <v>7288783</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>2</v>
       </c>
+      <c r="C15">
+        <v>1982586</v>
+      </c>
+      <c r="D15">
+        <v>2684126</v>
+      </c>
+      <c r="E15">
+        <v>2718830</v>
+      </c>
+      <c r="F15">
+        <v>2866032</v>
+      </c>
+      <c r="G15">
+        <v>7320912</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="C16">
+        <v>1969553</v>
+      </c>
+      <c r="D16">
+        <v>2632178</v>
+      </c>
+      <c r="E16">
+        <v>2702226</v>
+      </c>
+      <c r="F16">
+        <v>2917085</v>
+      </c>
+      <c r="G16">
+        <v>7180403</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="e">
+      <c r="C17" s="2">
         <f>SUM(C14:C16)/COUNT(C14:C16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="2" t="e">
+        <v>34.013644444444445</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" ref="D17:G17" si="5">SUM(D14:D16)/COUNT(D14:D16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="2" t="e">
+        <v>46.943350000000002</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="2" t="e">
+        <v>45.427411111111113</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="2" t="e">
+        <v>48.166966666666667</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>121.0561</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7068668</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2">
+        <v>7753235</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>3</v>
       </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="2">
+        <v>6905809</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -1625,9 +1847,9 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="2" t="e">
+      <c r="G21" s="2">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>120.70951111111113</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -1657,6 +1879,9 @@
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D25">
+        <v>1270394</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1674,6 +1899,9 @@
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D26">
+        <v>1850208</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1691,6 +1919,9 @@
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D27">
+        <v>1400298</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1709,9 +1940,9 @@
         <f>SUM(C25:C27)/COUNT(C25:C27)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="2" t="e">
+      <c r="D28" s="2">
         <f t="shared" ref="D28" si="7">SUM(D25:D27)/COUNT(D25:D27)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>25.116111111111113</v>
       </c>
       <c r="E28" s="2" t="e">
         <f t="shared" ref="E28" si="8">SUM(E25:E27)/COUNT(E25:E27)/1000/60</f>
@@ -1943,6 +2174,9 @@
       <c r="C43" t="s">
         <v>25</v>
       </c>
+      <c r="D43">
+        <v>2040257</v>
+      </c>
       <c r="E43" t="s">
         <v>25</v>
       </c>
@@ -1960,6 +2194,9 @@
       <c r="C44" t="s">
         <v>25</v>
       </c>
+      <c r="D44">
+        <v>2031705</v>
+      </c>
       <c r="E44" t="s">
         <v>25</v>
       </c>
@@ -1977,6 +2214,9 @@
       <c r="C45" t="s">
         <v>25</v>
       </c>
+      <c r="D45">
+        <v>2067626</v>
+      </c>
       <c r="E45" t="s">
         <v>25</v>
       </c>
@@ -1995,9 +2235,9 @@
         <f>SUM(C43:C45)/COUNT(C43:C45)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D46" s="2" t="e">
+      <c r="D46" s="2">
         <f t="shared" ref="D46:G46" si="19">SUM(D43:D45)/COUNT(D43:D45)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>34.108822222222223</v>
       </c>
       <c r="E46" s="2" t="e">
         <f t="shared" si="19"/>
@@ -2019,6 +2259,9 @@
       <c r="C47" t="s">
         <v>25</v>
       </c>
+      <c r="D47" s="2">
+        <v>1764978</v>
+      </c>
       <c r="E47" t="s">
         <v>25</v>
       </c>
@@ -2036,6 +2279,9 @@
       <c r="C48" t="s">
         <v>25</v>
       </c>
+      <c r="D48" s="2">
+        <v>1701382</v>
+      </c>
       <c r="E48" t="s">
         <v>25</v>
       </c>
@@ -2053,6 +2299,9 @@
       <c r="C49" t="s">
         <v>25</v>
       </c>
+      <c r="D49" s="2">
+        <v>1711224</v>
+      </c>
       <c r="E49" t="s">
         <v>25</v>
       </c>
@@ -2071,9 +2320,9 @@
         <f>SUM(C47:C49)/COUNT(C47:C49)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D50" s="2" t="e">
+      <c r="D50" s="2">
         <f t="shared" ref="D50:G50" si="20">SUM(D47:D49)/COUNT(D47:D49)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>28.764355555555554</v>
       </c>
       <c r="E50" s="2" t="e">
         <f t="shared" si="20"/>
@@ -2095,6 +2344,9 @@
       <c r="C51" t="s">
         <v>25</v>
       </c>
+      <c r="D51" s="2">
+        <v>2387376</v>
+      </c>
       <c r="E51" t="s">
         <v>25</v>
       </c>
@@ -2112,6 +2364,9 @@
       <c r="C52" t="s">
         <v>25</v>
       </c>
+      <c r="D52" s="2">
+        <v>2354064</v>
+      </c>
       <c r="E52" t="s">
         <v>25</v>
       </c>
@@ -2129,6 +2384,9 @@
       <c r="C53" t="s">
         <v>25</v>
       </c>
+      <c r="D53" s="2">
+        <v>2343043</v>
+      </c>
       <c r="E53" t="s">
         <v>25</v>
       </c>
@@ -2147,9 +2405,9 @@
         <f>SUM(C51:C53)/COUNT(C51:C53)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D54" s="2" t="e">
+      <c r="D54" s="2">
         <f t="shared" ref="D54:G54" si="21">SUM(D51:D53)/COUNT(D51:D53)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>39.358238888888891</v>
       </c>
       <c r="E54" s="2" t="e">
         <f t="shared" si="21"/>
@@ -2172,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FB19B8-25DC-1046-869A-DB575E87635F}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2215,6 +2473,12 @@
       <c r="D3">
         <v>12257</v>
       </c>
+      <c r="E3">
+        <v>39026</v>
+      </c>
+      <c r="F3">
+        <v>220701</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -2226,6 +2490,12 @@
       <c r="D4">
         <v>11553</v>
       </c>
+      <c r="E4">
+        <v>46871</v>
+      </c>
+      <c r="F4">
+        <v>265675</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -2237,6 +2507,12 @@
       <c r="D5">
         <v>11232</v>
       </c>
+      <c r="E5">
+        <v>46723</v>
+      </c>
+      <c r="F5">
+        <v>258856</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
@@ -2250,13 +2526,13 @@
         <f t="shared" ref="D6:G6" si="0">SUM(D3:D5)/COUNT(D3:D5)/1000/60</f>
         <v>0.19467777777777776</v>
       </c>
-      <c r="E6" s="2" t="e">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="2" t="e">
+        <v>0.73677777777777775</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4.1401777777777777</v>
       </c>
       <c r="G6" s="2" t="e">
         <f t="shared" si="0"/>
@@ -2273,6 +2549,12 @@
       <c r="D7" s="2">
         <v>10869</v>
       </c>
+      <c r="E7" s="2">
+        <v>55177</v>
+      </c>
+      <c r="F7" s="2">
+        <v>224288</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -2284,6 +2566,12 @@
       <c r="D8" s="2">
         <v>11129</v>
       </c>
+      <c r="E8" s="2">
+        <v>52786</v>
+      </c>
+      <c r="F8" s="2">
+        <v>275607</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -2295,6 +2583,12 @@
       <c r="D9" s="2">
         <v>12188</v>
       </c>
+      <c r="E9" s="2">
+        <v>51982</v>
+      </c>
+      <c r="F9" s="2">
+        <v>297293</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -2308,13 +2602,13 @@
         <f t="shared" ref="D10:G10" si="1">SUM(D7:D9)/COUNT(D7:D9)/1000/60</f>
         <v>0.18992222222222221</v>
       </c>
-      <c r="E10" s="2" t="e">
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="2" t="e">
+        <v>0.88858333333333328</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>4.4288222222222222</v>
       </c>
       <c r="G10" s="2" t="e">
         <f t="shared" si="1"/>
@@ -2345,56 +2639,146 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
+      <c r="C14">
+        <v>11252</v>
+      </c>
+      <c r="D14">
+        <v>9924</v>
+      </c>
+      <c r="E14">
+        <v>14213</v>
+      </c>
+      <c r="F14">
+        <v>59775</v>
+      </c>
+      <c r="G14">
+        <v>4239377</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>2</v>
       </c>
+      <c r="C15">
+        <v>11486</v>
+      </c>
+      <c r="D15">
+        <v>10034</v>
+      </c>
+      <c r="E15">
+        <v>15486</v>
+      </c>
+      <c r="F15">
+        <v>60278</v>
+      </c>
+      <c r="G15">
+        <v>4157173</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="C16">
+        <v>9846</v>
+      </c>
+      <c r="D16">
+        <v>7550</v>
+      </c>
+      <c r="E16">
+        <v>14232</v>
+      </c>
+      <c r="F16">
+        <v>59589</v>
+      </c>
+      <c r="G16">
+        <v>3949181</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="e">
+      <c r="C17" s="2">
         <f>SUM(C14:C16)/COUNT(C14:C16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="2" t="e">
+        <v>0.18102222222222225</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" ref="D17:G17" si="2">SUM(D14:D16)/COUNT(D14:D16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="2" t="e">
+        <v>0.15282222222222225</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="2" t="e">
+        <v>0.24406111111111112</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="2" t="e">
+        <v>0.99801111111111107</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>68.587394444444442</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4392261</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3723769</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>3</v>
       </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3958184</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -2416,9 +2800,9 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="2" t="e">
+      <c r="G21" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>67.078966666666659</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -2448,8 +2832,12 @@
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>25</v>
+      <c r="D25">
+        <v>8470</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25">
+        <v>223938</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>25</v>
@@ -2462,8 +2850,12 @@
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>25</v>
+      <c r="D26">
+        <v>9108</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26">
+        <v>262114</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>25</v>
@@ -2476,8 +2868,12 @@
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>25</v>
+      <c r="D27">
+        <v>8609</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27">
+        <v>186586</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>25</v>
@@ -2491,17 +2887,17 @@
         <f>SUM(C25:C27)/COUNT(C25:C27)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="2" t="e">
+      <c r="D28" s="2">
         <f t="shared" ref="D28:G28" si="4">SUM(D25:D27)/COUNT(D25:D27)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>0.14548333333333333</v>
       </c>
       <c r="E28" s="2" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="2" t="e">
+      <c r="F28" s="2">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>3.7368777777777775</v>
       </c>
       <c r="G28" s="2" t="e">
         <f t="shared" si="4"/>
@@ -2516,10 +2912,11 @@
         <v>25</v>
       </c>
       <c r="D29">
-        <v>7673</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>25</v>
+        <v>8653</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2">
+        <v>244744</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>25</v>
@@ -2533,10 +2930,11 @@
         <v>25</v>
       </c>
       <c r="D30">
-        <v>8210</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>7854</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2">
+        <v>247322</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>25</v>
@@ -2550,10 +2948,11 @@
         <v>25</v>
       </c>
       <c r="D31">
-        <v>8003</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>25</v>
+        <v>8168</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="2">
+        <v>250132</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>25</v>
@@ -2569,22 +2968,22 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32:G32" si="5">SUM(D29:D31)/COUNT(D29:D31)/1000/60</f>
-        <v>0.13269999999999998</v>
+        <v>0.13708333333333333</v>
       </c>
       <c r="E32" s="2" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F32" s="2" t="e">
+      <c r="F32" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>4.1233222222222228</v>
       </c>
       <c r="G32" s="2" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>11</v>
       </c>
@@ -2592,22 +2991,28 @@
         <v>12</v>
       </c>
       <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
         <v>13</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>14</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>15</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>1</v>
       </c>
+      <c r="C36">
+        <v>271684</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2617,11 +3022,17 @@
       <c r="G36" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>1</v>
       </c>
+      <c r="C37">
+        <v>307963</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2631,11 +3042,17 @@
       <c r="G37" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>1</v>
       </c>
+      <c r="C38">
+        <v>280120</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2645,21 +3062,24 @@
       <c r="G38" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="2" t="e">
+      <c r="C39" s="2">
         <f>SUM(C36:C38)/COUNT(C36:C38)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>4.7764833333333332</v>
       </c>
       <c r="D39" s="2" t="e">
-        <f t="shared" ref="D39:G39" si="6">SUM(D36:D38)/COUNT(D36:D38)/1000/60</f>
+        <f>SUM(D36:D38)/COUNT(D36:D38)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E39" s="2" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E39:H39" si="6">SUM(E36:E38)/COUNT(E36:E38)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F39" s="2" t="e">
@@ -2670,8 +3090,12 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>17</v>
       </c>
@@ -2691,40 +3115,58 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>22</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
       </c>
-      <c r="E43" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>9535</v>
+      </c>
+      <c r="F43">
+        <v>315197</v>
+      </c>
+      <c r="G43">
+        <v>3300691</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
       </c>
-      <c r="E44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>11384</v>
+      </c>
+      <c r="F44">
+        <v>283754</v>
+      </c>
+      <c r="G44">
+        <v>3458050</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>22</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
       </c>
-      <c r="E45" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>10903</v>
+      </c>
+      <c r="F45">
+        <v>311846</v>
+      </c>
+      <c r="G45">
+        <v>3352344</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>20</v>
       </c>
@@ -2732,43 +3174,55 @@
         <f>SUM(C43:C45)/COUNT(C43:C45)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D46" s="2" t="e">
+      <c r="D46" s="2">
         <f t="shared" ref="D46:G46" si="7">SUM(D43:D45)/COUNT(D43:D45)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>0.17678888888888888</v>
       </c>
       <c r="E46" s="2" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F46" s="2" t="e">
+      <c r="F46" s="2">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G46" s="2" t="e">
+        <v>5.0599833333333333</v>
+      </c>
+      <c r="G46" s="2">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+        <v>56.172694444444446</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>23</v>
       </c>
       <c r="C47" t="s">
         <v>25</v>
       </c>
-      <c r="E47" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D47" s="2">
+        <v>10687</v>
+      </c>
+      <c r="F47" s="2">
+        <v>236936</v>
+      </c>
+      <c r="G47" s="2">
+        <v>2579361</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>23</v>
       </c>
       <c r="C48" t="s">
         <v>25</v>
       </c>
-      <c r="E48" t="s">
-        <v>25</v>
+      <c r="D48" s="2">
+        <v>9530</v>
+      </c>
+      <c r="F48" s="2">
+        <v>274495</v>
+      </c>
+      <c r="G48" s="2">
+        <v>2951908</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
@@ -2778,8 +3232,14 @@
       <c r="C49" t="s">
         <v>25</v>
       </c>
-      <c r="E49" t="s">
-        <v>25</v>
+      <c r="D49" s="2">
+        <v>10440</v>
+      </c>
+      <c r="F49" s="2">
+        <v>258486</v>
+      </c>
+      <c r="G49" s="2">
+        <v>2905602</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
@@ -2790,21 +3250,21 @@
         <f>SUM(C47:C49)/COUNT(C47:C49)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D50" s="2" t="e">
+      <c r="D50" s="2">
         <f t="shared" ref="D50:G50" si="8">SUM(D47:D49)/COUNT(D47:D49)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>0.17031666666666664</v>
       </c>
       <c r="E50" s="2" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F50" s="2" t="e">
+      <c r="F50" s="2">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G50" s="2" t="e">
+        <v>4.2773166666666667</v>
+      </c>
+      <c r="G50" s="2">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>46.871505555555558</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
@@ -2814,8 +3274,14 @@
       <c r="C51" t="s">
         <v>25</v>
       </c>
-      <c r="E51" t="s">
-        <v>25</v>
+      <c r="D51" s="2">
+        <v>11079</v>
+      </c>
+      <c r="F51" s="2">
+        <v>301783</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2724657</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
@@ -2825,8 +3291,14 @@
       <c r="C52" t="s">
         <v>25</v>
       </c>
-      <c r="E52" t="s">
-        <v>25</v>
+      <c r="D52" s="2">
+        <v>10737</v>
+      </c>
+      <c r="F52" s="2">
+        <v>291015</v>
+      </c>
+      <c r="G52" s="2">
+        <v>3706707</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
@@ -2836,8 +3308,14 @@
       <c r="C53" t="s">
         <v>25</v>
       </c>
-      <c r="E53" t="s">
-        <v>25</v>
+      <c r="D53" s="2">
+        <v>11409</v>
+      </c>
+      <c r="F53" s="2">
+        <v>301051</v>
+      </c>
+      <c r="G53" s="2">
+        <v>2964525</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
@@ -2848,21 +3326,21 @@
         <f>SUM(C51:C53)/COUNT(C51:C53)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D54" s="2" t="e">
+      <c r="D54" s="2">
         <f t="shared" ref="D54:G54" si="9">SUM(D51:D53)/COUNT(D51:D53)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>0.18458333333333332</v>
       </c>
       <c r="E54" s="2" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F54" s="2" t="e">
+      <c r="F54" s="2">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G54" s="2" t="e">
+        <v>4.9658277777777782</v>
+      </c>
+      <c r="G54" s="2">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>52.199383333333337</v>
       </c>
     </row>
   </sheetData>
@@ -2874,8 +3352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7998DB6-1797-544D-9A8B-84492D5AC6D8}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2921,6 +3399,15 @@
       <c r="D3">
         <v>2354</v>
       </c>
+      <c r="E3">
+        <v>17820</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -2932,6 +3419,15 @@
       <c r="D4">
         <v>2294</v>
       </c>
+      <c r="E4">
+        <v>17741</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -2943,6 +3439,15 @@
       <c r="D5">
         <v>2345</v>
       </c>
+      <c r="E5">
+        <v>17562</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
@@ -2956,9 +3461,9 @@
         <f t="shared" ref="D6:G6" si="0">SUM(D3:D5)/COUNT(D3:D5)/1000/60</f>
         <v>3.8850000000000003E-2</v>
       </c>
-      <c r="E6" s="2" t="e">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.29512777777777782</v>
       </c>
       <c r="F6" s="2" t="e">
         <f t="shared" si="0"/>
@@ -2979,6 +3484,15 @@
       <c r="D7" s="2">
         <v>37948</v>
       </c>
+      <c r="E7" s="2">
+        <v>3599197</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -2990,6 +3504,15 @@
       <c r="D8" s="2">
         <v>37697</v>
       </c>
+      <c r="E8" s="2">
+        <v>3853275</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -3001,6 +3524,15 @@
       <c r="D9" s="2">
         <v>38286</v>
       </c>
+      <c r="E9" s="2">
+        <v>3603600</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -3014,9 +3546,9 @@
         <f t="shared" ref="D10:G10" si="1">SUM(D7:D9)/COUNT(D7:D9)/1000/60</f>
         <v>0.6329499999999999</v>
       </c>
-      <c r="E10" s="2" t="e">
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>61.422622222222223</v>
       </c>
       <c r="F10" s="2" t="e">
         <f t="shared" si="1"/>
@@ -3051,28 +3583,46 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
+      <c r="C14">
+        <v>2326</v>
+      </c>
+      <c r="D14">
+        <v>2885</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>2</v>
       </c>
+      <c r="C15">
+        <v>2359</v>
+      </c>
+      <c r="D15">
+        <v>2924</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="C16">
+        <v>2532</v>
+      </c>
+      <c r="D16">
+        <v>2763</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="e">
+      <c r="C17" s="2">
         <f>SUM(C14:C16)/COUNT(C14:C16)/1000/60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="2" t="e">
+        <v>4.009444444444444E-2</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" ref="D17:G17" si="2">SUM(D14:D16)/COUNT(D14:D16)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>4.7622222222222226E-2</v>
       </c>
       <c r="E17" s="2" t="e">
         <f t="shared" si="2"/>
@@ -3091,16 +3641,52 @@
       <c r="B18" t="s">
         <v>3</v>
       </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>3</v>
       </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -3154,7 +3740,13 @@
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D25">
+        <v>1277</v>
+      </c>
       <c r="E25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -3168,7 +3760,11 @@
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26">
+        <v>1283</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -3182,7 +3778,11 @@
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="D27">
+        <v>1343</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -3197,9 +3797,9 @@
         <f>SUM(C25:C27)/COUNT(C25:C27)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D28" s="2" t="e">
+      <c r="D28" s="2">
         <f t="shared" ref="D28:G28" si="4">SUM(D25:D27)/COUNT(D25:D27)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>2.1683333333333332E-2</v>
       </c>
       <c r="E28" s="2" t="e">
         <f t="shared" si="4"/>
@@ -3224,7 +3824,8 @@
       <c r="D29">
         <v>1347</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -3241,7 +3842,8 @@
       <c r="D30">
         <v>1358</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -3258,7 +3860,8 @@
       <c r="D31">
         <v>1339</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -3314,6 +3917,12 @@
       <c r="B36" t="s">
         <v>1</v>
       </c>
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>25</v>
       </c>
@@ -3328,6 +3937,12 @@
       <c r="B37" t="s">
         <v>1</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>25</v>
       </c>
@@ -3342,6 +3957,12 @@
       <c r="B38" t="s">
         <v>1</v>
       </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>25</v>
       </c>
@@ -3404,7 +4025,13 @@
       <c r="C43" t="s">
         <v>25</v>
       </c>
-      <c r="E43" t="s">
+      <c r="D43">
+        <v>2283</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3415,7 +4042,13 @@
       <c r="C44" t="s">
         <v>25</v>
       </c>
-      <c r="E44" t="s">
+      <c r="D44">
+        <v>2282</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3426,7 +4059,13 @@
       <c r="C45" t="s">
         <v>25</v>
       </c>
-      <c r="E45" t="s">
+      <c r="D45">
+        <v>2344</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3438,9 +4077,9 @@
         <f>SUM(C43:C45)/COUNT(C43:C45)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D46" s="2" t="e">
+      <c r="D46" s="2">
         <f t="shared" ref="D46:G46" si="7">SUM(D43:D45)/COUNT(D43:D45)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>3.8383333333333332E-2</v>
       </c>
       <c r="E46" s="2" t="e">
         <f t="shared" si="7"/>
@@ -3462,7 +4101,13 @@
       <c r="C47" t="s">
         <v>25</v>
       </c>
-      <c r="E47" t="s">
+      <c r="D47" s="2">
+        <v>2146</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3473,7 +4118,13 @@
       <c r="C48" t="s">
         <v>25</v>
       </c>
-      <c r="E48" t="s">
+      <c r="D48" s="2">
+        <v>2081</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3484,7 +4135,13 @@
       <c r="C49" t="s">
         <v>25</v>
       </c>
-      <c r="E49" t="s">
+      <c r="D49" s="2">
+        <v>2087</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3496,9 +4153,9 @@
         <f>SUM(C47:C49)/COUNT(C47:C49)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D50" s="2" t="e">
+      <c r="D50" s="2">
         <f t="shared" ref="D50:G50" si="8">SUM(D47:D49)/COUNT(D47:D49)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>3.5077777777777777E-2</v>
       </c>
       <c r="E50" s="2" t="e">
         <f t="shared" si="8"/>
@@ -3520,7 +4177,13 @@
       <c r="C51" t="s">
         <v>25</v>
       </c>
-      <c r="E51" t="s">
+      <c r="D51" s="2">
+        <v>2088</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3531,7 +4194,13 @@
       <c r="C52" t="s">
         <v>25</v>
       </c>
-      <c r="E52" t="s">
+      <c r="D52" s="2">
+        <v>2082</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3542,7 +4211,13 @@
       <c r="C53" t="s">
         <v>25</v>
       </c>
-      <c r="E53" t="s">
+      <c r="D53" s="2">
+        <v>2082</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3554,9 +4229,9 @@
         <f>SUM(C51:C53)/COUNT(C51:C53)/1000/60</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D54" s="2" t="e">
+      <c r="D54" s="2">
         <f t="shared" ref="D54:G54" si="9">SUM(D51:D53)/COUNT(D51:D53)/1000/60</f>
-        <v>#DIV/0!</v>
+        <v>3.4733333333333331E-2</v>
       </c>
       <c r="E54" s="2" t="e">
         <f t="shared" si="9"/>

</xml_diff>